<commit_message>
I think a few small serializer changes.
</commit_message>
<xml_diff>
--- a/respondents/static/respondents/upload-template.xlsx
+++ b/respondents/static/respondents/upload-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jay_r\bonaso-data-portal\bonaso_data_server\respondents\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jay_r\bonaso-data-portal\bonaso_data_server\respondents\static\respondents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC0FAC3-461A-498F-82D6-81B9DFD2AD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B54783-97F9-423A-989A-38DEED4D8D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{B81ECF7F-CEA6-4A1A-96A5-3B694CAE9AEE}"/>
   </bookViews>
@@ -35,11 +35,236 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+  <si>
+    <t>Welcome to the Report Generation Template</t>
+  </si>
+  <si>
+    <t>If this is your first time, please take a moment to go through the instructions.</t>
+  </si>
+  <si>
+    <t>1. Purpose</t>
+  </si>
+  <si>
+    <t>The purpose of this template is to allow you to upload large amounts of data at once. We understand that it may take time for you to completely shift to online reporting, and offer this tool as a way to "bridge the gap." This way, if you or any of your partners still need to collect data on paper or in Excel, you do not have to enter each entry manually.</t>
+  </si>
+  <si>
+    <t>2. Instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you download the template, it already has all the fields you need, including all the demographic information about your clients and all the tasks/indicators that your organization (or your child organization) has been assigned. So you should be ready to start recording data immediately. However, please take a moment to read through the tips below for the best and easiest experience. </t>
+  </si>
+  <si>
+    <t>Respondent Demographic Information</t>
+  </si>
+  <si>
+    <t>General Tips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The above fields will appear on every template. It is information that we need to collect about the people we work with for our data analysis. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A quick note about </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Is Anonymous</t>
+    </r>
+  </si>
+  <si>
+    <t>We understand that sometimes the people you work with may not want to provide sensitive information about themselves. That's why we give the option to create an "anonymous respondent" that requires less information. However, please note that we still need some information to collect valid data. Please take a moment to compare the two respondents below, the one in the first row is not anonymous, while the one in the second is.</t>
+  </si>
+  <si>
+    <t>Required Fields if anonymous:</t>
+  </si>
+  <si>
+    <t>Age Range</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Citizenship/Nationality</t>
+  </si>
+  <si>
+    <t>Required Fields if not anonymous</t>
+  </si>
+  <si>
+    <t>ID Number</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Key population status, disability status, and ward are optional for both anonymous and non anonymous.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email and phone number are optional as well, but we request you do not provide this information if a respondent wishes to remain anonymous. </t>
+  </si>
+  <si>
+    <t>Check the dropdowns!</t>
+  </si>
+  <si>
+    <t>Before you start recording any data, make sure you check the dropdown options. You can do this by clicking on the row just beneath the header and looking for a little arrow.</t>
+  </si>
+  <si>
+    <t>If you see a dropdown field, that means that whatever you enter into this cell must match one or more of the options below.</t>
+  </si>
+  <si>
+    <t>THIS IS IMPORTANT</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For the fields </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Key Population Status, Disability Status, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and any indicator that is not a number and does not have yes/no as its options, you can select multiple values from the list.</t>
+    </r>
+  </si>
+  <si>
+    <t>To do this, just separate each value with a comma</t>
+  </si>
+  <si>
+    <t>Another Example</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If you do not match your cell content to the dropdown exactly, when you go to upload, you will get an error. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>You must match the spelling exactly for it to work.</t>
+    </r>
+  </si>
+  <si>
+    <t>Requires a Number</t>
+  </si>
+  <si>
+    <t>This means the task is expecting a number (i.e., Number of Condoms Distributed).</t>
+  </si>
+  <si>
+    <t>If you do not provide a number, you will get an error</t>
+  </si>
+  <si>
+    <r>
+      <t>Some tasks will have a "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Requires a Number)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" next to the column name.</t>
+    </r>
+  </si>
+  <si>
+    <t>Can I leave it blank?</t>
+  </si>
+  <si>
+    <t>Aside from the respondent fields (see above) and the interaction date, anything else can be left blank.</t>
+  </si>
+  <si>
+    <t>If you, for example, have a column header for "Tested for HIV", but the person was not tested, you can leave it blank, and it will be ignored when you upload.</t>
+  </si>
+  <si>
+    <t>I got an error, what now?</t>
+  </si>
+  <si>
+    <t>The error should tell you what happened and where. Some common culprits may include an incorrect date value, accidently leaving something blank, or not matching the dropdown options exactly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you get an error, that does not mean your upload entirely failed. Just the select records. You can edit your file to fix the issue and upload again. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just note that you may get </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you left a task/indicator blank, you may get a warning. If this was intentional, you can safely ignore it. </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -66,8 +291,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -83,6 +333,231 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>197424</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171478</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61B74DB7-0369-CFD3-B46C-CA8811D0011C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4235450"/>
+          <a:ext cx="11170224" cy="539778"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>178373</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>95283</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{143D4E71-5E01-8FA4-E5EE-E49B9D97AEB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5892800"/>
+          <a:ext cx="11151173" cy="647733"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>135107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>176462</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>105114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{930F333D-C580-471C-BBA4-6C153212D8A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10896330"/>
+          <a:ext cx="5040292" cy="881975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>116268</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>2046</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABA488DA-57D8-A035-6E92-6AF291DBA87C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12609132"/>
+          <a:ext cx="11063310" cy="1099881"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>491149</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>70555</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4F63428-47E5-4C54-36EF-A0BA2C13A471}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="13705417"/>
+          <a:ext cx="11444899" cy="1181805"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,14 +877,637 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D88FFA-0D1E-4EDE-ACE3-5D674670AC18}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="94" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A58" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+      <c r="M82" s="2"/>
+      <c r="N82" s="2"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A87" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" s="2"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A92" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2"/>
+      <c r="N92" s="2"/>
+      <c r="O92" s="2"/>
+      <c r="P92" s="2"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A55:Q55"/>
+    <mergeCell ref="A82:N82"/>
+    <mergeCell ref="A87:O87"/>
+    <mergeCell ref="A92:P92"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A14:I20"/>
+    <mergeCell ref="A24:P24"/>
+    <mergeCell ref="A21:P21"/>
+    <mergeCell ref="A30:R32"/>
+    <mergeCell ref="A29:R29"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="A4:E5"/>
+    <mergeCell ref="A8:I12"/>
+    <mergeCell ref="A7:I7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Slight issue with file upload perms.
</commit_message>
<xml_diff>
--- a/respondents/static/respondents/upload-template.xlsx
+++ b/respondents/static/respondents/upload-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\bonaso_data_portal\bonaso_data_server\respondents\static\respondents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E747BEC9-EA41-4CE0-A180-D7D206A4559F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C4B0E3-C55D-40B8-AA18-03D92AAFC937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8" yWindow="8" windowWidth="20505" windowHeight="13065" xr2:uid="{B81ECF7F-CEA6-4A1A-96A5-3B694CAE9AEE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{B81ECF7F-CEA6-4A1A-96A5-3B694CAE9AEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="116">
   <si>
     <t>Welcome to the Report Generation Template</t>
   </si>
@@ -493,6 +493,56 @@
   </si>
   <si>
     <t>BAD! Separate each category with a comma.</t>
+  </si>
+  <si>
+    <t>Select from the dropdown</t>
+  </si>
+  <si>
+    <t>Type name of village (primary/current residence)</t>
+  </si>
+  <si>
+    <t>Select from the dropdown (primary/current residence)</t>
+  </si>
+  <si>
+    <t>Type the name of the country this person is from (e.g. Botswana, Zimbabwe)</t>
+  </si>
+  <si>
+    <t>Respondents Omang/Passport Number</t>
+  </si>
+  <si>
+    <t>Type the date that this person was born at.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please use the dropdowns when selecting Key Population status, disability status, and special respondent status. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note that you can select multiple options for these categories</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, if they are seperated by a comma.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">You can also enter HIV Data and pregnancy data for any respondent. Just make sure for HIV Status you enter  the date this person was positive (or today's date if you are unsure). </t>
+  </si>
+  <si>
+    <t>For pregnancies, you can record an active pregnancy or the person's most recent pregnancy. Make sure you put the date the person's term began, and if the pregnancy has conlcuded, the date that it ended.</t>
   </si>
 </sst>
 </file>
@@ -579,7 +629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -588,59 +638,20 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -648,15 +659,42 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -997,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D88FFA-0D1E-4EDE-ACE3-5D674670AC18}">
-  <dimension ref="A1:W107"/>
+  <dimension ref="A1:W109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="94" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1023,225 +1061,225 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
@@ -1273,24 +1311,24 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
@@ -1298,232 +1336,232 @@
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="I26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K26" s="10" t="s">
+      <c r="K26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L26" s="10" t="s">
+      <c r="L26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M26" s="10" t="s">
+      <c r="M26" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N26" s="10" t="s">
+      <c r="N26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O26" s="10" t="s">
+      <c r="O26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P26" s="10" t="s">
+      <c r="P26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q26" s="10" t="s">
+      <c r="Q26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="R26" s="10" t="s">
+      <c r="R26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="S26" s="10" t="s">
+      <c r="S26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="T26" s="10" t="s">
+      <c r="T26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="U26" s="10" t="s">
+      <c r="U26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V26" s="10" t="s">
+      <c r="V26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="W26" s="10"/>
+      <c r="W26" s="4"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I33" s="10" t="s">
+      <c r="I33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J33" s="10" t="s">
+      <c r="J33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K33" s="10" t="s">
+      <c r="K33" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L33" s="10" t="s">
+      <c r="L33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M33" s="10" t="s">
+      <c r="M33" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N33" s="10" t="s">
+      <c r="N33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O33" s="10" t="s">
+      <c r="O33" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P33" s="10" t="s">
+      <c r="P33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Q33" s="10" t="s">
+      <c r="Q33" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="R33" s="10" t="s">
+      <c r="R33" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="S33" s="10" t="s">
+      <c r="S33" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="T33" s="10" t="s">
+      <c r="T33" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="U33" s="10" t="s">
+      <c r="U33" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V33" s="10" t="s">
+      <c r="V33" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="W33" s="10"/>
+      <c r="W33" s="4"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A34" t="b">
         <v>1</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C34" t="s">
@@ -1532,7 +1570,7 @@
       <c r="D34" t="s">
         <v>54</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F34" s="5">
         <v>36749</v>
       </c>
       <c r="G34" t="s">
@@ -1553,10 +1591,10 @@
       <c r="L34" t="s">
         <v>59</v>
       </c>
-      <c r="M34" s="12" t="s">
+      <c r="M34" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="N34" s="13" t="s">
+      <c r="N34" s="7" t="s">
         <v>61</v>
       </c>
       <c r="O34" t="s">
@@ -1571,10 +1609,10 @@
       <c r="S34" t="s">
         <v>65</v>
       </c>
-      <c r="T34" s="11">
+      <c r="T34" s="5">
         <v>45515</v>
       </c>
-      <c r="U34" s="11">
+      <c r="U34" s="5">
         <v>45880</v>
       </c>
     </row>
@@ -1608,50 +1646,68 @@
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>9</v>
       </c>
+      <c r="C38" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
         <v>10</v>
       </c>
+      <c r="C39" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>11</v>
       </c>
+      <c r="C40" s="4" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
         <v>12</v>
       </c>
+      <c r="C41" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>13</v>
       </c>
+      <c r="C42" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
         <v>15</v>
       </c>
+      <c r="C45" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
@@ -1667,543 +1723,562 @@
       <c r="B48" t="s">
         <v>11</v>
       </c>
+      <c r="C48" s="4" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
         <v>12</v>
       </c>
+      <c r="C49" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
         <v>13</v>
       </c>
+      <c r="C50" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
         <v>18</v>
       </c>
+      <c r="C51" s="4" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7"/>
-      <c r="O52" s="7"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
+      <c r="M52" s="21"/>
+      <c r="N52" s="21"/>
+      <c r="O52" s="21"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
+      <c r="M53" s="21"/>
+      <c r="N53" s="21"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A55" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
+      <c r="A55" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A57" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="14"/>
+      <c r="N57" s="14"/>
+      <c r="O57" s="14"/>
+      <c r="P57" s="14"/>
+      <c r="Q57" s="14"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A58" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A60" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A61" s="10" t="s">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A63" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A62" s="14" t="s">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A64" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="B64" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A63" s="34" t="s">
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="23"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A65" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B63" s="31" t="s">
+      <c r="B65" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A65" s="4" t="s">
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="24"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A67" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A66" s="4" t="s">
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="14"/>
+      <c r="N67" s="14"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A68" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A67" s="15" t="s">
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="14"/>
+      <c r="L68" s="14"/>
+      <c r="M68" s="14"/>
+      <c r="N68" s="14"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A69" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B67" s="15"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A68" s="16" t="s">
+      <c r="B69" s="25"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A70" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="B68" s="16"/>
-      <c r="C68" s="18" t="s">
+      <c r="B70" s="26"/>
+      <c r="C70" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
-      <c r="J68" s="17"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A69" s="32" t="s">
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A71" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B69" s="32"/>
-      <c r="C69" s="33" t="s">
+      <c r="B71" s="27"/>
+      <c r="C71" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="34"/>
-      <c r="H69" s="34"/>
-      <c r="I69" s="34"/>
-      <c r="J69" s="34"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A74" s="3" t="s">
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A76" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A75" s="7" t="s">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A77" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A76" s="16" t="s">
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A78" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B76" s="16"/>
-      <c r="C76" s="16"/>
-      <c r="D76" s="16"/>
-      <c r="E76" s="16"/>
-      <c r="F76" s="21" t="s">
+      <c r="B78" s="26"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
+      <c r="E78" s="26"/>
+      <c r="F78" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="G76" s="21"/>
-      <c r="H76" s="21"/>
-      <c r="I76" s="21"/>
-      <c r="J76" s="21"/>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A77" s="32" t="s">
+      <c r="G78" s="28"/>
+      <c r="H78" s="28"/>
+      <c r="I78" s="28"/>
+      <c r="J78" s="28"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A79" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="B77" s="32"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="32"/>
-      <c r="F77" s="31" t="s">
+      <c r="B79" s="27"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="27"/>
+      <c r="E79" s="27"/>
+      <c r="F79" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="G77" s="31"/>
-      <c r="H77" s="31"/>
-      <c r="I77" s="31"/>
-      <c r="J77" s="31"/>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A78" s="32" t="s">
+      <c r="G79" s="24"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+      <c r="J79" s="24"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A80" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B78" s="32"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="32"/>
-      <c r="E78" s="32"/>
-      <c r="F78" s="31" t="s">
+      <c r="B80" s="27"/>
+      <c r="C80" s="27"/>
+      <c r="D80" s="27"/>
+      <c r="E80" s="27"/>
+      <c r="F80" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="G78" s="31"/>
-      <c r="H78" s="31"/>
-      <c r="I78" s="31"/>
-      <c r="J78" s="31"/>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A81" s="4" t="s">
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="24"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A83" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="4"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
-      <c r="N81" s="4"/>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
-        <v>90</v>
-      </c>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="14"/>
+      <c r="N83" s="14"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A85" s="3" t="s">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A87" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A86" s="10" t="s">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A88" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A87" s="20">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A89" s="9">
         <v>6</v>
       </c>
-      <c r="B87" s="18" t="s">
+      <c r="B89" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C87" s="17"/>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A88" s="30" t="s">
+      <c r="C89" s="9"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A90" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="31" t="s">
+      <c r="B90" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="C88" s="31"/>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A89" s="24" t="s">
+      <c r="C90" s="24"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A91" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B89" s="24"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24"/>
-      <c r="G89" s="24"/>
-      <c r="H89" s="24"/>
-      <c r="I89" s="24"/>
-      <c r="J89" s="24"/>
-      <c r="K89" s="24"/>
-      <c r="L89" s="24"/>
-      <c r="M89" s="24"/>
-      <c r="N89" s="24"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A90" s="22" t="s">
+      <c r="B91" s="14"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
+      <c r="L91" s="14"/>
+      <c r="M91" s="14"/>
+      <c r="N91" s="14"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
         <v>95</v>
       </c>
-      <c r="B90" s="23"/>
-      <c r="C90" s="23"/>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A91" s="22" t="s">
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
         <v>96</v>
       </c>
-      <c r="B91" s="23"/>
-      <c r="C91" s="23"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A92" s="25" t="s">
+      <c r="B93" s="11"/>
+      <c r="C93" s="11"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A94" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="B92" s="25"/>
-      <c r="C92" s="25"/>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A93" s="26" t="s">
+      <c r="B94" s="25"/>
+      <c r="C94" s="25"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A95" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B93" s="26"/>
-      <c r="C93" s="26"/>
-      <c r="D93" s="27" t="s">
+      <c r="B95" s="26"/>
+      <c r="C95" s="26"/>
+      <c r="D95" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="27"/>
-      <c r="H93" s="27"/>
-      <c r="I93" s="27"/>
-      <c r="J93" s="27"/>
-      <c r="K93" s="27"/>
-      <c r="L93" s="27"/>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A94" s="28" t="s">
+      <c r="E95" s="17"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="17"/>
+      <c r="H95" s="17"/>
+      <c r="I95" s="17"/>
+      <c r="J95" s="17"/>
+      <c r="K95" s="17"/>
+      <c r="L95" s="17"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A96" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="29" t="s">
+      <c r="B96" s="15"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E94" s="29"/>
-      <c r="F94" s="29"/>
-      <c r="G94" s="29"/>
-      <c r="H94" s="29"/>
-      <c r="I94" s="29"/>
-      <c r="J94" s="29"/>
-      <c r="K94" s="29"/>
-      <c r="L94" s="29"/>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A95" s="28" t="s">
+      <c r="E96" s="16"/>
+      <c r="F96" s="16"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="16"/>
+      <c r="I96" s="16"/>
+      <c r="J96" s="16"/>
+      <c r="K96" s="16"/>
+      <c r="L96" s="16"/>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A97" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B95" s="28"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="29" t="s">
+      <c r="B97" s="15"/>
+      <c r="C97" s="15"/>
+      <c r="D97" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="E95" s="29"/>
-      <c r="F95" s="29"/>
-      <c r="G95" s="29"/>
-      <c r="H95" s="29"/>
-      <c r="I95" s="29"/>
-      <c r="J95" s="29"/>
-      <c r="K95" s="29"/>
-      <c r="L95" s="29"/>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A96" s="28" t="s">
+      <c r="E97" s="16"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="16"/>
+      <c r="H97" s="16"/>
+      <c r="I97" s="16"/>
+      <c r="J97" s="16"/>
+      <c r="K97" s="16"/>
+      <c r="L97" s="16"/>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A98" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B96" s="28"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="29" t="s">
+      <c r="B98" s="15"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="E96" s="29"/>
-      <c r="F96" s="29"/>
-      <c r="G96" s="29"/>
-      <c r="H96" s="29"/>
-      <c r="I96" s="29"/>
-      <c r="J96" s="29"/>
-      <c r="K96" s="29"/>
-      <c r="L96" s="29"/>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="B97" s="23"/>
-      <c r="C97" s="23"/>
-    </row>
-    <row r="98" spans="1:16" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="4" t="s">
+      <c r="E98" s="16"/>
+      <c r="F98" s="16"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="16"/>
+      <c r="I98" s="16"/>
+      <c r="J98" s="16"/>
+      <c r="K98" s="16"/>
+      <c r="L98" s="16"/>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="B99" s="11"/>
+      <c r="C99" s="11"/>
+    </row>
+    <row r="100" spans="1:16" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A100" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="4"/>
-      <c r="G98" s="4"/>
-      <c r="H98" s="4"/>
-      <c r="I98" s="4"/>
-      <c r="J98" s="4"/>
-      <c r="K98" s="4"/>
-      <c r="L98" s="4"/>
-      <c r="M98" s="4"/>
-      <c r="N98" s="4"/>
-      <c r="O98" s="4"/>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A99" s="4" t="s">
+      <c r="B100" s="14"/>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="14"/>
+      <c r="G100" s="14"/>
+      <c r="H100" s="14"/>
+      <c r="I100" s="14"/>
+      <c r="J100" s="14"/>
+      <c r="K100" s="14"/>
+      <c r="L100" s="14"/>
+      <c r="M100" s="14"/>
+      <c r="N100" s="14"/>
+      <c r="O100" s="14"/>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A101" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
-      <c r="G99" s="4"/>
-      <c r="H99" s="4"/>
-      <c r="I99" s="4"/>
-      <c r="J99" s="4"/>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A100" s="4" t="s">
+      <c r="B101" s="14"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14"/>
+      <c r="H101" s="14"/>
+      <c r="I101" s="14"/>
+      <c r="J101" s="14"/>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A102" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
-      <c r="I100" s="4"/>
-      <c r="J100" s="4"/>
-      <c r="K100" s="4"/>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A103" s="4" t="s">
+      <c r="B102" s="14"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="14"/>
+      <c r="I102" s="14"/>
+      <c r="J102" s="14"/>
+      <c r="K102" s="14"/>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A105" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="4"/>
-      <c r="J103" s="4"/>
-      <c r="K103" s="4"/>
-      <c r="L103" s="4"/>
-      <c r="M103" s="4"/>
-      <c r="N103" s="4"/>
-      <c r="O103" s="4"/>
-      <c r="P103" s="4"/>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A104" t="s">
-        <v>33</v>
-      </c>
+      <c r="B105" s="14"/>
+      <c r="C105" s="14"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="14"/>
+      <c r="G105" s="14"/>
+      <c r="H105" s="14"/>
+      <c r="I105" s="14"/>
+      <c r="J105" s="14"/>
+      <c r="K105" s="14"/>
+      <c r="L105" s="14"/>
+      <c r="M105" s="14"/>
+      <c r="N105" s="14"/>
+      <c r="O105" s="14"/>
+      <c r="P105" s="14"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A107" t="s">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A99:J99"/>
-    <mergeCell ref="A100:K100"/>
+    <mergeCell ref="A95:C95"/>
+    <mergeCell ref="F79:J79"/>
+    <mergeCell ref="F80:J80"/>
+    <mergeCell ref="F78:J78"/>
+    <mergeCell ref="A91:N91"/>
     <mergeCell ref="A94:C94"/>
-    <mergeCell ref="A95:C95"/>
-    <mergeCell ref="A96:C96"/>
-    <mergeCell ref="D94:L94"/>
-    <mergeCell ref="D93:L93"/>
-    <mergeCell ref="D95:L95"/>
-    <mergeCell ref="D96:L96"/>
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="A4:E5"/>
-    <mergeCell ref="A8:I12"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A52:O52"/>
-    <mergeCell ref="A103:P103"/>
+    <mergeCell ref="A105:P105"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="A14:I20"/>
     <mergeCell ref="A24:P24"/>
@@ -2211,29 +2286,37 @@
     <mergeCell ref="A30:R32"/>
     <mergeCell ref="A29:R29"/>
     <mergeCell ref="A53:N53"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="A65:N65"/>
-    <mergeCell ref="A66:N66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B65:G65"/>
+    <mergeCell ref="A67:N67"/>
+    <mergeCell ref="A68:N68"/>
     <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
     <mergeCell ref="A37:D37"/>
+    <mergeCell ref="D95:L95"/>
+    <mergeCell ref="D97:L97"/>
+    <mergeCell ref="D98:L98"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="A4:E5"/>
+    <mergeCell ref="A8:I12"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A52:O52"/>
     <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A55:Q55"/>
-    <mergeCell ref="A81:N81"/>
-    <mergeCell ref="A98:O98"/>
-    <mergeCell ref="A76:E76"/>
+    <mergeCell ref="A57:Q57"/>
+    <mergeCell ref="A83:N83"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="A79:E79"/>
+    <mergeCell ref="A80:E80"/>
     <mergeCell ref="A77:E77"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="A75:E75"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="F77:J77"/>
-    <mergeCell ref="F78:J78"/>
-    <mergeCell ref="F76:J76"/>
-    <mergeCell ref="A89:N89"/>
-    <mergeCell ref="A92:C92"/>
-    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="A101:J101"/>
+    <mergeCell ref="A102:K102"/>
+    <mergeCell ref="A96:C96"/>
+    <mergeCell ref="A97:C97"/>
+    <mergeCell ref="A98:C98"/>
+    <mergeCell ref="D96:L96"/>
+    <mergeCell ref="A100:O100"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M34" r:id="rId1" xr:uid="{89770CAC-BFCF-4CF9-A942-6F3625516CFB}"/>

</xml_diff>